<commit_message>
LambdaMapping - backtest to StrategyBase.xlsx updated: allow_entry_initial|final mapped to allow_entry_initial|final
</commit_message>
<xml_diff>
--- a/siglab_py/LambdaMapping - backtest to StrategyBase.xlsx
+++ b/siglab_py/LambdaMapping - backtest to StrategyBase.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\siglab\siglab_py\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEF8D62-7F6A-47D6-8F18-D777AA9D8433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18612270-CF21-4B60-97A8-15EF959E37D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="-1965" windowWidth="19380" windowHeight="10260" xr2:uid="{64FB003A-71C9-4620-8FE1-FA72144932C7}"/>
+    <workbookView xWindow="-17100" yWindow="-170" windowWidth="12110" windowHeight="8375" xr2:uid="{64FB003A-71C9-4620-8FE1-FA72144932C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>allow_entry_final</t>
   </si>
   <si>
-    <t>allow_entry</t>
-  </si>
-  <si>
     <t>order_notional_adj</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>StrategyBase</t>
+  </si>
+  <si>
+    <t>allow_entry_init</t>
   </si>
 </sst>
 </file>
@@ -472,7 +472,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -483,10 +483,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -494,10 +494,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -508,7 +508,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,7 +519,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -527,10 +527,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -538,10 +538,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -549,10 +549,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -560,10 +560,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -571,13 +571,14 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>